<commit_message>
Adding Columns in review log
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2250" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
-  <si>
-    <t>Source</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Comment</t>
   </si>
@@ -109,13 +106,31 @@
   <si>
     <t>SRS IDs not cleat enough; you have just write CRS ids inside it.
 You have to translate/convert CRS to technical SRS and give every requirement in SRS an ID</t>
+  </si>
+  <si>
+    <t>Resolver</t>
+  </si>
+  <si>
+    <t>Resolved in version number</t>
+  </si>
+  <si>
+    <t>Document Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Review Date</t>
+  </si>
+  <si>
+    <t>Resolving Date</t>
+  </si>
+  <si>
+    <t>Review Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +165,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,6 +209,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -281,6 +305,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -315,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,177 +516,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="33" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="31.5703125" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="23.25">
+    <row r="1" spans="1:12" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="61.5" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -668,7 +714,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -676,7 +722,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -684,7 +730,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -692,7 +738,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -700,7 +746,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -708,7 +754,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -716,7 +762,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -724,7 +770,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -732,7 +778,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -740,7 +786,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -748,7 +794,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -756,7 +802,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -764,7 +810,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -772,7 +818,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -780,7 +826,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -788,7 +834,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -796,7 +842,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -804,7 +850,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -812,7 +858,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -820,7 +866,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -828,7 +874,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -836,7 +882,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -844,7 +890,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -852,7 +898,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -860,7 +906,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -868,7 +914,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -876,7 +922,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -884,7 +930,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -892,7 +938,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -900,7 +946,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -908,7 +954,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -916,7 +962,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -924,7 +970,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -932,7 +978,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -940,7 +986,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -948,7 +994,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -956,7 +1002,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -964,7 +1010,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -972,7 +1018,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -980,7 +1026,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>

</xml_diff>

<commit_message>
Adding Columns in review log (reverted from commit 4c3ceea9b018c8bc29afbea1440215debdda132f)
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+  <si>
+    <t>Source</t>
+  </si>
   <si>
     <t>Comment</t>
   </si>
@@ -106,31 +109,13 @@
   <si>
     <t>SRS IDs not cleat enough; you have just write CRS ids inside it.
 You have to translate/convert CRS to technical SRS and give every requirement in SRS an ID</t>
-  </si>
-  <si>
-    <t>Resolver</t>
-  </si>
-  <si>
-    <t>Resolved in version number</t>
-  </si>
-  <si>
-    <t>Document Version</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Review Date</t>
-  </si>
-  <si>
-    <t>Resolving Date</t>
-  </si>
-  <si>
-    <t>Review Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +150,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -187,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,9 +188,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -305,7 +281,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -340,7 +315,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -516,197 +490,177 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" customWidth="1"/>
-    <col min="11" max="11" width="38.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="23.25">
       <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="61.5" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75">
       <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -714,7 +668,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -722,7 +676,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -730,7 +684,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -738,7 +692,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -746,7 +700,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -754,7 +708,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -762,7 +716,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -770,7 +724,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -778,7 +732,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -786,7 +740,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -794,7 +748,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -802,7 +756,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -810,7 +764,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -818,7 +772,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -826,7 +780,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -834,7 +788,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -842,7 +796,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -850,7 +804,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -858,7 +812,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -866,7 +820,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -874,7 +828,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -882,7 +836,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -890,7 +844,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -898,7 +852,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -906,7 +860,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -914,7 +868,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -922,7 +876,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -930,7 +884,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -938,7 +892,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -946,7 +900,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -954,7 +908,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -962,7 +916,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -970,7 +924,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -978,7 +932,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -986,7 +940,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -994,7 +948,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1002,7 +956,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1010,7 +964,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1018,7 +972,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1026,7 +980,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>

</xml_diff>

<commit_message>
Adding Columns to review log
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
-  <si>
-    <t>Source</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Comment</t>
   </si>
@@ -109,13 +106,28 @@
   <si>
     <t>SRS IDs not cleat enough; you have just write CRS ids inside it.
 You have to translate/convert CRS to technical SRS and give every requirement in SRS an ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Review Date</t>
+  </si>
+  <si>
+    <t>Review Status</t>
+  </si>
+  <si>
+    <t>Resolver</t>
+  </si>
+  <si>
+    <t>Resolving Date</t>
+  </si>
+  <si>
+    <t>Document Version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +162,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -166,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -188,6 +206,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -281,6 +302,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -315,6 +337,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -490,14 +513,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -506,161 +529,177 @@
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="23.25">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75">
-      <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="61.5" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -668,7 +707,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -676,7 +715,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -684,7 +723,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -692,7 +731,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -700,7 +739,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -708,7 +747,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -716,7 +755,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -724,7 +763,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -732,7 +771,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -740,7 +779,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -748,7 +787,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -756,7 +795,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -764,7 +803,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -772,7 +811,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -780,7 +819,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -788,7 +827,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -796,7 +835,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -804,7 +843,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -812,7 +851,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -820,7 +859,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -828,7 +867,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -836,7 +875,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -844,7 +883,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -852,7 +891,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -860,7 +899,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -868,7 +907,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -876,7 +915,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -884,7 +923,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -892,7 +931,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -900,7 +939,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -908,7 +947,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -916,7 +955,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -924,7 +963,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -932,7 +971,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -940,7 +979,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -948,7 +987,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -956,7 +995,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -964,7 +1003,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -972,7 +1011,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -980,7 +1019,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>

</xml_diff>

<commit_message>
Adding New Reviews Issues
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Comment</t>
   </si>
@@ -145,6 +145,30 @@
   </si>
   <si>
     <t>v1.0</t>
+  </si>
+  <si>
+    <t>REV_007</t>
+  </si>
+  <si>
+    <t>TEST_PLN</t>
+  </si>
+  <si>
+    <t>Eng. Mohamed Hassan</t>
+  </si>
+  <si>
+    <t>REV_008</t>
+  </si>
+  <si>
+    <t>Items Not to be Tested,Features not to be tested, Need to be removed because they are not in the project scope</t>
+  </si>
+  <si>
+    <t>Review strategy need to be included for the items need to be tested</t>
+  </si>
+  <si>
+    <t>REV_009</t>
+  </si>
+  <si>
+    <t>Regression Test Need To be more Clarified</t>
   </si>
 </sst>
 </file>
@@ -231,11 +255,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,7 +568,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,8 +586,8 @@
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -718,7 +742,7 @@
       <c r="G6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="J6" s="6" t="s">
@@ -750,7 +774,7 @@
       <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>39</v>
       </c>
       <c r="J7" s="6" t="s">
@@ -782,7 +806,7 @@
       <c r="G8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -792,32 +816,85 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>

</xml_diff>

<commit_message>
Adding new Review issues
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="54">
   <si>
     <t>Comment</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Regression Test Need To be more Clarified</t>
+  </si>
+  <si>
+    <t>REV_010</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>Severity Criteria need to be defined</t>
   </si>
 </sst>
 </file>
@@ -567,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,11 +904,30 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>

</xml_diff>

<commit_message>
SRS was reviewed by Basma and the findings were logged in the review log Basma Emad
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
   <si>
     <t>Comment</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>15/4/2018</t>
+  </si>
+  <si>
+    <t>REV_011</t>
+  </si>
+  <si>
+    <t>Technical Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basma </t>
   </si>
 </sst>
 </file>
@@ -336,7 +345,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,7 +380,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,12 +963,24 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>

</xml_diff>

<commit_message>
SRS was reviewed by Basma and the findings were logged in the review log.
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
   <si>
     <t>Comment</t>
   </si>
@@ -193,6 +193,14 @@
   </si>
   <si>
     <t xml:space="preserve">Basma </t>
+  </si>
+  <si>
+    <t>16/4/2018</t>
+  </si>
+  <si>
+    <t>1- The Motor Driver as per requirement from the customer should be included in SRS
+2- The Short, Long and frequent press should be cleared in SRS
+3- "Motor rotational speed will be evaluated based on sight and sound as per requested by the customer" should be included in SRS</t>
   </si>
 </sst>
 </file>
@@ -256,16 +264,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -284,6 +286,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,672 +608,678 @@
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="41.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" customWidth="1"/>
     <col min="10" max="10" width="24.42578125" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="G13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Closed the logged case in the review log regarding the SRS
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2256" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
   <si>
     <t>Comment</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t xml:space="preserve">1-API's naming convention not followed as in naming convention doucment </t>
+  </si>
+  <si>
+    <t>khaled hossam</t>
+  </si>
+  <si>
+    <t>17/4/2018</t>
   </si>
 </sst>
 </file>
@@ -223,7 +229,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -231,7 +237,7 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -239,7 +245,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3" tint="0.39997558519241921"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -299,11 +305,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -365,7 +371,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -400,7 +406,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -611,31 +617,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="24.625" customWidth="1"/>
-    <col min="3" max="3" width="32.25" customWidth="1"/>
-    <col min="4" max="4" width="28.25" customWidth="1"/>
-    <col min="5" max="5" width="21.75" customWidth="1"/>
-    <col min="6" max="6" width="19.25" customWidth="1"/>
-    <col min="7" max="7" width="41.625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.125" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="10" width="24.375" customWidth="1"/>
-    <col min="11" max="11" width="23.25" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -670,7 +676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -702,7 +708,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -734,7 +740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -766,7 +772,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -796,7 +802,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -828,7 +834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -860,7 +866,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -895,7 +901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -921,7 +927,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -956,7 +962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -982,7 +988,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1007,8 +1013,17 @@
       <c r="H13" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="I13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -1030,11 +1045,11 @@
       <c r="G14" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>43206</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1042,7 +1057,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1050,7 +1065,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1058,7 +1073,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1066,7 +1081,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1074,7 +1089,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1082,7 +1097,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1090,7 +1105,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1098,7 +1113,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1106,7 +1121,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1114,7 +1129,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1122,7 +1137,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1130,7 +1145,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1138,7 +1153,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1146,7 +1161,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1154,7 +1169,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1162,7 +1177,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1170,7 +1185,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1178,7 +1193,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1186,7 +1201,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1194,7 +1209,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1202,7 +1217,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1210,7 +1225,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1218,7 +1233,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1226,7 +1241,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1234,7 +1249,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1242,7 +1257,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1250,7 +1265,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1258,7 +1273,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1266,7 +1281,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1274,7 +1289,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1282,7 +1297,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1290,7 +1305,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1298,7 +1313,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1306,7 +1321,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>

</xml_diff>

<commit_message>
Logging result of reviewing Project Milestones , Criteria for determining severity By : Marwan Ahmed Thabet
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2256" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
   <si>
     <t>Comment</t>
   </si>
@@ -219,13 +219,29 @@
   </si>
   <si>
     <t>17/4/2018</t>
+  </si>
+  <si>
+    <t>TEST_PLN =&gt; Criteria for determining severity</t>
+  </si>
+  <si>
+    <t>Marwan Ahmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- The document title should be more descriptive please make it  "Criteria for determining severity" instead of "Severity"
+2- The mentioned Criteria are general please make them more specific and related  to our project </t>
+  </si>
+  <si>
+    <t>Project Milesontes</t>
+  </si>
+  <si>
+    <t>RTM should be in a separate task not connected to Design document so make a task card for RTM and another two cards for high level design and component design documents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,7 +387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,10 +419,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,7 +453,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -614,34 +628,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
-    <col min="7" max="7" width="41.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -676,7 +690,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="61.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -708,7 +722,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="45">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -740,7 +754,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -772,7 +786,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="30">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -802,7 +816,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="75">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -834,7 +848,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="75">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -866,7 +880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -901,7 +915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="30">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -927,7 +941,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -962,7 +976,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -988,7 +1002,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="129" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1023,7 +1037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="30">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -1049,23 +1063,49 @@
         <v>43206</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="90">
       <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="75">
       <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1073,7 +1113,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1081,7 +1121,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1089,7 +1129,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1097,7 +1137,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1105,7 +1145,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1113,7 +1153,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1121,7 +1161,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1129,7 +1169,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1137,7 +1177,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1145,7 +1185,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1153,7 +1193,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1161,7 +1201,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1169,7 +1209,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1177,7 +1217,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1185,7 +1225,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1193,7 +1233,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1201,7 +1241,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1209,7 +1249,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1217,7 +1257,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1225,7 +1265,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1233,7 +1273,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1241,7 +1281,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1249,7 +1289,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1257,7 +1297,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1265,7 +1305,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1273,7 +1313,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1281,7 +1321,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1289,7 +1329,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1297,7 +1337,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1305,7 +1345,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1313,7 +1353,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1321,7 +1361,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>

</xml_diff>

<commit_message>
SRS was reviewed by Basma and Ahmed Raafat and the findings were logged in the review log
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
   <si>
     <t>Comment</t>
   </si>
@@ -235,13 +235,28 @@
   </si>
   <si>
     <t>RTM should be in a separate task not connected to Design document so make a task card for RTM and another two cards for high level design and component design documents</t>
+  </si>
+  <si>
+    <t>18/4/2018</t>
+  </si>
+  <si>
+    <t>Basma and Ahmed Raafat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- [SRS _9] Frequent button press is described as button pressing and releasing in interval less than 1/3 second. It should mention what will be happened 
+2- [SRS _4] Motor operating voltage is between 5 to 9V.  It should specify that the motor will work in this range only otherwise it will be off
+3- Feature 2: Power supply should be connected to the motor to provide voltage either inside or outside the voltage range.
+ower supply should be connected to the motor driver not motor directly.
+4- Feature 2: The SIQ suggested using fuse to control the overvoltage state instead of the HW protection circuit.
+5- Feature2: You can’t assume that the motor voltage is stable and it should be protected also by a fuse as stated in SIQ updates, also don’t use the term hw protection circuit as it may be fuse. 
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,7 +402,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,9 +434,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -453,6 +469,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -628,20 +645,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="7" max="7" width="41.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
@@ -650,12 +667,12 @@
     <col min="11" max="11" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.25">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18.75">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -690,7 +707,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="61.5" customHeight="1">
+    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -722,7 +739,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -754,7 +771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -786,7 +803,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30">
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -816,7 +833,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="75">
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -848,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="75">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -880,7 +897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="45">
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -915,7 +932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -941,7 +958,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -976,7 +993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1002,7 +1019,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129" customHeight="1">
+    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1010,7 +1027,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>57</v>
@@ -1037,7 +1054,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="30">
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -1063,7 +1080,7 @@
         <v>43206</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="90">
+    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
         <v>67</v>
@@ -1084,7 +1101,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="75">
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>70</v>
@@ -1105,15 +1122,31 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1121,7 +1154,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1129,7 +1162,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1137,7 +1170,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1145,7 +1178,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1153,7 +1186,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1161,7 +1194,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1169,7 +1202,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1177,7 +1210,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1185,7 +1218,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1193,7 +1226,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1201,7 +1234,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1209,7 +1242,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1217,7 +1250,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1225,7 +1258,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1233,7 +1266,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1241,7 +1274,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1249,7 +1282,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1257,7 +1290,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1265,7 +1298,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1273,7 +1306,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1281,7 +1314,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1289,7 +1322,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1297,7 +1330,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1305,7 +1338,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1313,7 +1346,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1321,7 +1354,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1329,7 +1362,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1337,7 +1370,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1345,7 +1378,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1353,7 +1386,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1361,7 +1394,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>

</xml_diff>

<commit_message>
Resolving log regarding SRS requirements
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2256" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
   <si>
     <t>Comment</t>
   </si>
@@ -281,6 +281,12 @@
 3/interfaces(services) has no description
 4/naming convention not met
 </t>
+  </si>
+  <si>
+    <t>Khaled hossam</t>
+  </si>
+  <si>
+    <t>Resolved</t>
   </si>
 </sst>
 </file>
@@ -291,7 +297,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -299,7 +305,7 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -307,7 +313,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3" tint="0.39997558519241921"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -370,12 +376,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,7 +443,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,7 +478,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,31 +689,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
-    <col min="2" max="2" width="24.75" customWidth="1"/>
-    <col min="3" max="3" width="32.25" customWidth="1"/>
-    <col min="4" max="4" width="28.25" customWidth="1"/>
-    <col min="5" max="5" width="25.125" customWidth="1"/>
-    <col min="6" max="6" width="19.25" customWidth="1"/>
-    <col min="7" max="7" width="41.75" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.125" customWidth="1"/>
-    <col min="9" max="9" width="23.25" customWidth="1"/>
-    <col min="10" max="10" width="24.25" customWidth="1"/>
-    <col min="11" max="11" width="23.25" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="32.21875" customWidth="1"/>
+    <col min="4" max="4" width="28.21875" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="7" max="7" width="41.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.21875" customWidth="1"/>
+    <col min="10" max="10" width="24.21875" customWidth="1"/>
+    <col min="11" max="11" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -742,7 +748,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -774,7 +780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -806,7 +812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -838,7 +844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -868,7 +874,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -900,7 +906,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -932,7 +938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -967,7 +973,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -993,7 +999,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -1028,7 +1034,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -1124,7 +1130,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
         <v>67</v>
@@ -1145,7 +1151,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="57" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>70</v>
@@ -1166,7 +1172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="299.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="288" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1188,8 +1194,17 @@
       <c r="H17" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="9">
+        <v>43210</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>77</v>
       </c>
@@ -1217,14 +1232,14 @@
       <c r="I18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="9">
         <v>43209</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>81</v>
       </c>
@@ -1252,14 +1267,14 @@
       <c r="I19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="10">
         <v>43209</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1267,7 +1282,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1275,7 +1290,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1283,7 +1298,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1291,7 +1306,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1299,7 +1314,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1307,7 +1322,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1315,7 +1330,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1323,7 +1338,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1331,7 +1346,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1339,7 +1354,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1347,7 +1362,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1355,7 +1370,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1363,7 +1378,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1371,7 +1386,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1379,7 +1394,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1387,7 +1402,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1395,7 +1410,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1403,7 +1418,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1411,7 +1426,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1419,7 +1434,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1427,7 +1442,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1435,7 +1450,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1443,7 +1458,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1451,7 +1466,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1459,7 +1474,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1467,7 +1482,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1475,7 +1490,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1483,7 +1498,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1491,7 +1506,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>

</xml_diff>

<commit_message>
Opening new log regarding HLD_4 design document
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -287,6 +287,17 @@
   </si>
   <si>
     <t>Resolved</t>
+  </si>
+  <si>
+    <t>REV_17</t>
+  </si>
+  <si>
+    <t>HLD_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- The table of contents should be relevant to the doc contents.
+2- The covers item in table 3.1.1 and 3.1.2 is not consistent with the covers item in the interface table, Its value is CDD_N while it should be changed to HLD_N
+</t>
   </si>
 </sst>
 </file>
@@ -689,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,13 +1285,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+    <row r="20" spans="1:11" ht="127.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="9">
+        <v>43210</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>

</xml_diff>

<commit_message>
resolved REV_17 on HLD_4
</commit_message>
<xml_diff>
--- a/management/Review-Log.xlsx
+++ b/management/Review-Log.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2256" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2250" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="89">
   <si>
     <t>Comment</t>
   </si>
@@ -308,7 +308,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -316,7 +316,7 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -324,7 +324,7 @@
       <b/>
       <sz val="18"/>
       <color theme="3" tint="0.39997558519241921"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -454,7 +454,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -489,7 +489,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,31 +700,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F28" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="32.21875" customWidth="1"/>
-    <col min="4" max="4" width="28.21875" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
-    <col min="7" max="7" width="41.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.109375" customWidth="1"/>
-    <col min="9" max="9" width="23.21875" customWidth="1"/>
-    <col min="10" max="10" width="24.21875" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="2" max="2" width="24.75" customWidth="1"/>
+    <col min="3" max="3" width="32.25" customWidth="1"/>
+    <col min="4" max="4" width="28.25" customWidth="1"/>
+    <col min="5" max="5" width="25.125" customWidth="1"/>
+    <col min="6" max="6" width="19.25" customWidth="1"/>
+    <col min="7" max="7" width="41.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.125" customWidth="1"/>
+    <col min="9" max="9" width="23.25" customWidth="1"/>
+    <col min="10" max="10" width="24.25" customWidth="1"/>
+    <col min="11" max="11" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -759,7 +759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -791,7 +791,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -823,7 +823,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -855,7 +855,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -885,7 +885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
@@ -917,7 +917,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -949,7 +949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
@@ -984,7 +984,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>51</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>56</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="6" t="s">
         <v>67</v>
@@ -1162,7 +1162,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="57" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>70</v>
@@ -1183,7 +1183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="288" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="299.25" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>77</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>81</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="127.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="127.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>86</v>
       </c>
@@ -1310,8 +1310,17 @@
       <c r="H20" s="9">
         <v>43210</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="9">
+        <v>43210</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1319,7 +1328,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1327,7 +1336,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1335,7 +1344,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1343,7 +1352,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1351,7 +1360,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1359,7 +1368,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1367,7 +1376,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1375,7 +1384,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1383,7 +1392,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1391,7 +1400,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1399,7 +1408,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1407,7 +1416,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1415,7 +1424,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1423,7 +1432,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1431,7 +1440,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1439,7 +1448,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1447,7 +1456,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1455,7 +1464,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1463,7 +1472,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1471,7 +1480,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1479,7 +1488,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1487,7 +1496,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1495,7 +1504,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1503,7 +1512,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1511,7 +1520,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1519,7 +1528,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1527,7 +1536,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1535,7 +1544,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>

</xml_diff>